<commit_message>
Changes texts in web
</commit_message>
<xml_diff>
--- a/VotingSystem_2b/src/main/test/resourceselecciones.xlsx
+++ b/VotingSystem_2b/src/main/test/resourceselecciones.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nauce\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="15030" windowHeight="3690"/>
   </bookViews>
@@ -12,59 +17,52 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Partido</t>
-  </si>
-  <si>
-    <t>NIF</t>
-  </si>
-  <si>
-    <t>AA</t>
-  </si>
-  <si>
-    <t>BB</t>
-  </si>
-  <si>
-    <t>CC</t>
-  </si>
-  <si>
-    <t>11111111A</t>
-  </si>
-  <si>
-    <t>22222222B</t>
-  </si>
-  <si>
-    <t>33333333C</t>
-  </si>
-  <si>
-    <t>Alberto</t>
-  </si>
-  <si>
-    <t>Borja</t>
-  </si>
-  <si>
-    <t>Carlos</t>
-  </si>
-  <si>
-    <t>Apellido</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>Alvarez</t>
-  </si>
-  <si>
-    <t>Baston</t>
-  </si>
-  <si>
-    <t>Cienfuegos</t>
+    <t>Inicial</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Descripcion1</t>
+  </si>
+  <si>
+    <t>Descripcion2</t>
+  </si>
+  <si>
+    <t>Descripcion3</t>
+  </si>
+  <si>
+    <t>Partido Socialista</t>
+  </si>
+  <si>
+    <t>PSOE</t>
+  </si>
+  <si>
+    <t>Partido Popular</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>Podemos</t>
+  </si>
+  <si>
+    <t>Ciudadanos</t>
+  </si>
+  <si>
+    <t>C's</t>
+  </si>
+  <si>
+    <t>Descripcion4</t>
   </si>
 </sst>
 </file>
@@ -112,6 +110,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -159,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,7 +195,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -403,69 +404,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>